<commit_message>
Got simple keyboard commands to run model-train working fixed bug in modbus master regarding shift directio of data to be written to modbusslave registers.
to do:
- read back current consumtion etc via ADC and apply filtering, only averaging done now (LPF via ADC^2)
- create piggy back for occupied signal detection and read this signal also with filter and check
  if occupied signal can be determined.
- create regulator etc when occupied signal is set, amplifier will ramp down.
- try to drive 2 trains on 3 sections (or assamble the 4th modbus slave)
- build 1 backplane slave for automatic slave insertion via modbus master to all slaves
</commit_message>
<xml_diff>
--- a/TrackAmplifier3.X/doc/Baudrate calc.xlsx
+++ b/TrackAmplifier3.X/doc/Baudrate calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-REPOS\Siebwalde\TrackAmplifier3.X\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{001DFA25-5864-401F-9056-389E0B49A1E1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E145D76F-9343-4733-AA34-63604F86E3A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12795" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12795" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Fosc</t>
   </si>
@@ -142,6 +142,27 @@
   </si>
   <si>
     <t>HW @3,23</t>
+  </si>
+  <si>
+    <t>INA326</t>
+  </si>
+  <si>
+    <t>INA180 A4</t>
+  </si>
+  <si>
+    <t>200V/V</t>
+  </si>
+  <si>
+    <t>Gain INA180</t>
+  </si>
+  <si>
+    <t>via compare gaat niet via Fvr met DAC laagste setting is 0,128V</t>
+  </si>
+  <si>
+    <t>Rechtstreeks inlezen op ADC kan, bij 10mA geeft dat 0,050V --&gt; 10 bits op de ADC.</t>
+  </si>
+  <si>
+    <t>ADC kan zelf filteren en via threshold trigger het signaal checken.</t>
   </si>
 </sst>
 </file>
@@ -2047,7 +2068,7 @@
   <dimension ref="A1:D259"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:C13"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5420,8 +5441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F0C607-2732-46DF-9DB7-EA90AC20C8B5}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5471,15 +5492,15 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B32" si="0">$A4*7.36</f>
+        <f t="shared" ref="B4:B17" si="0">$A4*7.36</f>
         <v>14.72</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C32" si="1">($A4*2.98)+36.28</f>
+        <f t="shared" ref="C4:C17" si="1">($A4*2.98)+36.28</f>
         <v>42.24</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D32" si="2">($A4*3.23)+36.28</f>
+        <f t="shared" ref="D4:D17" si="2">($A4*3.23)+36.28</f>
         <v>42.74</v>
       </c>
     </row>
@@ -5712,10 +5733,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C3:G11"/>
+  <dimension ref="C2:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5725,9 +5746,23 @@
     <col min="4" max="4" width="9.140625" style="7"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="7"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -5740,8 +5775,20 @@
       <c r="G3" s="7">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="7">
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="N3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -5754,8 +5801,20 @@
       <c r="G4" s="8">
         <v>5000</v>
       </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
@@ -5768,8 +5827,20 @@
       <c r="G5" s="8">
         <v>3.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>12</v>
       </c>
@@ -5777,8 +5848,16 @@
         <f>((D3-D4)*(D5/32))+ D4</f>
         <v>2.8159999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="7">
+        <f>((L3-L4)*(L5/32))+ L4</f>
+        <v>0.128</v>
+      </c>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -5793,10 +5872,37 @@
         <f>G3*G5*G4+2.5</f>
         <v>2.875</v>
       </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="7">
+        <f>L6</f>
+        <v>0.128</v>
+      </c>
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="7">
+        <f>O3*O5*O4</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>13</v>
+      </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>